<commit_message>
se agrego script enviar email
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seba\Desktop\dev\trabajo\editpdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E65D54-2E8E-4E4D-B17C-2E6386577653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A88ACCE-042C-4729-80D9-7EA95B074216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Dia</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Primario</t>
   </si>
   <si>
-    <t>sonietb5@gmail.com</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>ESCUELA PROVINCIAL Nº 9 - COMANDANTE LUIS PIEDRA BUENA</t>
   </si>
   <si>
-    <t>andres.am223@gmail.com</t>
-  </si>
-  <si>
     <t>ORUE</t>
   </si>
   <si>
@@ -109,7 +103,7 @@
     <t>ESCUELA PROVINCIAL Nº 15 - CENTENARIO DE USHUAIA</t>
   </si>
   <si>
-    <t>roorue98@gmail.com</t>
+    <t>sebastiandev.img@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -119,7 +113,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-2C0A]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -135,6 +129,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -174,10 +174,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -191,8 +192,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,9 +554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2088" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A388" sqref="A388:XFD2112"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,11 +650,11 @@
       <c r="K2" s="2">
         <v>45953</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>20</v>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -669,16 +674,16 @@
         <v>37479235</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>19</v>
@@ -686,11 +691,11 @@
       <c r="K3" s="2">
         <v>45967</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
+      <c r="L3" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -710,16 +715,16 @@
         <v>40828900</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>19</v>
@@ -727,11 +732,11 @@
       <c r="K4" s="2">
         <v>45958</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
+      <c r="L4" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -32340,9 +32345,14 @@
       <c r="M2111" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{93D1CCA4-F08E-4577-8A97-BB6D65277D6E}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{6C459E3E-8912-4085-AB59-E610EA34552D}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{47A560B5-C4A3-45AB-948D-E5B77B3F6BFC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>